<commit_message>
20170810T2213 - Other Economic and finanacial requirements
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="540" windowWidth="11355" windowHeight="6615" tabRatio="884" firstSheet="8" activeTab="15"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
-    <sheet name="ResponseDataType" sheetId="185" r:id="rId2"/>
-    <sheet name="AmountType" sheetId="178" r:id="rId3"/>
-    <sheet name="ConfidentialityLevel" sheetId="199" r:id="rId4"/>
-    <sheet name="ContractType" sheetId="144" r:id="rId5"/>
-    <sheet name="CountryCodeIdentifier" sheetId="190" r:id="rId6"/>
-    <sheet name="CriterionElementType" sheetId="202" r:id="rId7"/>
+    <sheet name="AmountType" sheetId="178" r:id="rId2"/>
+    <sheet name="ConfidentialityLevel" sheetId="199" r:id="rId3"/>
+    <sheet name="ContractType" sheetId="144" r:id="rId4"/>
+    <sheet name="CountryCodeIdentifier" sheetId="190" r:id="rId5"/>
+    <sheet name="CriterionElementType" sheetId="202" r:id="rId6"/>
+    <sheet name="ResponseDataType" sheetId="185" r:id="rId7"/>
     <sheet name="CriteriaType" sheetId="193" r:id="rId8"/>
     <sheet name="CurrencyCode" sheetId="191" r:id="rId9"/>
     <sheet name="DocRefContentType" sheetId="192" r:id="rId10"/>
@@ -36,7 +36,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="7">CriteriaType!$A$1:$C$75</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:A23"/>
 </workbook>
 </file>
 
@@ -6844,14 +6845,11 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22805" name="Table783713621145522170522806" displayName="Table783713621145522170522806" ref="A12:B35" totalsRowShown="0">
-  <autoFilter ref="A12:B35"/>
-  <sortState ref="A13:B23">
-    <sortCondition ref="A13"/>
-  </sortState>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16245" name="Table783716246" displayName="Table783716246" ref="A12:B18" totalsRowShown="0">
+  <autoFilter ref="A12:B18"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="32"/>
-    <tableColumn id="2" name="Value" dataDxfId="31"/>
+    <tableColumn id="1" name="Code" dataDxfId="30"/>
+    <tableColumn id="2" name="Value" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6919,17 +6917,6 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16245" name="Table783716246" displayName="Table783716246" ref="A12:B18" totalsRowShown="0">
-  <autoFilter ref="A12:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="30"/>
-    <tableColumn id="2" name="Value" dataDxfId="29"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24302" name="Table759524303" displayName="Table759524303" ref="A12:B14" tableType="xml" totalsRowShown="0" connectionId="63">
   <autoFilter ref="A12:B14"/>
   <tableColumns count="2">
@@ -6944,7 +6931,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7595" name="Table7595" displayName="Table7595" ref="A12:B20" tableType="xml" totalsRowShown="0" connectionId="63">
   <autoFilter ref="A12:B20"/>
   <tableColumns count="2">
@@ -6959,7 +6946,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="25037" name="Table759525038" displayName="Table759525038" ref="A12:B23" tableType="xml" totalsRowShown="0" connectionId="63">
   <autoFilter ref="A12:B23"/>
   <tableColumns count="2">
@@ -6969,6 +6956,20 @@
     <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="26">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22805" name="Table783713621145522170522806" displayName="Table783713621145522170522806" ref="A12:B35" totalsRowShown="0">
+  <autoFilter ref="A12:B35"/>
+  <sortState ref="A13:B23">
+    <sortCondition ref="A13"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Code" dataDxfId="32"/>
+    <tableColumn id="2" name="Value" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8464,7 +8465,7 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
       <selection sqref="A1:IV65536"/>
     </sheetView>
   </sheetViews>
@@ -9466,7 +9467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -10105,42 +10106,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <sheetPr codeName="Sheet21">
+    <tabColor theme="0" tint="-0.34998626667073579"/>
+  </sheetPr>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="175.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>268</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -10148,7 +10149,7 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -10156,7 +10157,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -10164,13 +10165,13 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -10178,7 +10179,7 @@
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -10186,7 +10187,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -10194,202 +10195,141 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>279</v>
+        <v>260</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>280</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>281</v>
+        <v>261</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>282</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>283</v>
+        <v>267</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>284</v>
+        <v>264</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>285</v>
+        <v>248</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>286</v>
+        <v>250</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>288</v>
-      </c>
+      <c r="A19" s="8"/>
+      <c r="B19" s="4"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>290</v>
-      </c>
+      <c r="A20" s="8"/>
+      <c r="B20" s="4"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>291</v>
-      </c>
+      <c r="A21" s="8"/>
+      <c r="B21" s="4"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>292</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>293</v>
-      </c>
+      <c r="A22" s="8"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>295</v>
-      </c>
+      <c r="A23" s="8"/>
+      <c r="B23" s="4"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>296</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>297</v>
-      </c>
+      <c r="A24" s="8"/>
+      <c r="B24" s="4"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>1271</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>1272</v>
-      </c>
+      <c r="A25" s="8"/>
+      <c r="B25" s="4"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>1316</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>1317</v>
-      </c>
+      <c r="A26" s="8"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>1406</v>
-      </c>
+      <c r="A27" s="8"/>
+      <c r="B27" s="4"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>1441</v>
-      </c>
+      <c r="A28" s="8"/>
+      <c r="B28" s="4"/>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
-        <v>1430</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>1442</v>
-      </c>
+      <c r="A29" s="8"/>
+      <c r="B29" s="4"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>1440</v>
-      </c>
+      <c r="A30" s="8"/>
+      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>1432</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>1439</v>
-      </c>
+      <c r="A31" s="8"/>
+      <c r="B31" s="4"/>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>1433</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>1438</v>
-      </c>
+      <c r="A32" s="8"/>
+      <c r="B32" s="4"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>1434</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>1436</v>
-      </c>
+      <c r="A33" s="8"/>
+      <c r="B33" s="4"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
-        <v>1435</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>1437</v>
-      </c>
+      <c r="A34" s="8"/>
+      <c r="B34" s="4"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>1443</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>1444</v>
-      </c>
+      <c r="A35" s="8"/>
+      <c r="B35" s="4"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="8"/>
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="8"/>
+      <c r="B37" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -11576,236 +11516,6 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet21">
-    <tabColor theme="0" tint="-0.34998626667073579"/>
-  </sheetPr>
-  <dimension ref="A1:B37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>1458</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>264</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>248</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="20" t="s">
-        <v>250</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="8"/>
-      <c r="B19" s="4"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="8"/>
-      <c r="B20" s="4"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="8"/>
-      <c r="B21" s="4"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="8"/>
-      <c r="B22" s="4"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="8"/>
-      <c r="B23" s="4"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="8"/>
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="8"/>
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="8"/>
-      <c r="B26" s="4"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="8"/>
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="8"/>
-      <c r="B28" s="4"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="8"/>
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="8"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="8"/>
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="8"/>
-      <c r="B32" s="4"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="8"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="8"/>
-      <c r="B34" s="4"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="8"/>
-      <c r="B35" s="4"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="8"/>
-      <c r="B36" s="4"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11928,7 +11638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:B20"/>
@@ -12095,7 +11805,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B262"/>
   <sheetViews>
@@ -14204,7 +13914,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -14400,6 +14110,297 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="175.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>273</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>292</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>296</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>1406</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B29" s="37" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
@@ -14407,7 +14408,7 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
20170821T2320 - Selection all, but pending wiki review.
- Harmonisation of data structures
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -37,7 +37,6 @@
     <definedName name="_xlnm.Print_Area" localSheetId="7">CriteriaType!$A$1:$C$75</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:A23"/>
 </workbook>
 </file>
 
@@ -5715,6 +5714,25 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -5783,25 +5801,6 @@
         <name val="Arial"/>
         <scheme val="none"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -6848,8 +6847,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16245" name="Table783716246" displayName="Table783716246" ref="A12:B18" totalsRowShown="0">
   <autoFilter ref="A12:B18"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="30"/>
-    <tableColumn id="2" name="Value" dataDxfId="29"/>
+    <tableColumn id="1" name="Code" dataDxfId="32"/>
+    <tableColumn id="2" name="Value" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6923,7 +6922,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="28">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="30">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6938,7 +6937,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="27">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="29">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6953,7 +6952,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="26">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="28">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6968,8 +6967,8 @@
     <sortCondition ref="A13"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="32"/>
-    <tableColumn id="2" name="Value" dataDxfId="31"/>
+    <tableColumn id="1" name="Code" dataDxfId="27"/>
+    <tableColumn id="2" name="Value" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -14114,7 +14113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14408,8 +14407,8 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
20170829T0026 - ESPD Response
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="5" activeTab="6"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -5297,24 +5297,6 @@
     <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -5332,6 +5314,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5413,19 +5413,19 @@
       </font>
     </dxf>
     <dxf>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -8447,7 +8447,7 @@
       <c r="A17" t="s">
         <v>1304</v>
       </c>
-      <c r="B17" s="34" t="s">
+      <c r="B17" s="28" t="s">
         <v>1305</v>
       </c>
     </row>
@@ -8464,8 +8464,8 @@
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9883,7 +9883,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9975,7 +9975,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="36">
+      <c r="A13" s="30">
         <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -9983,7 +9983,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="36">
+      <c r="A14" s="30">
         <v>2</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -9991,7 +9991,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="36">
+      <c r="A15" s="30">
         <v>3</v>
       </c>
       <c r="B15" s="1" t="s">
@@ -9999,7 +9999,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="36" t="s">
+      <c r="A16" s="30" t="s">
         <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -10007,7 +10007,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="36">
+      <c r="A17" s="30">
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -10015,7 +10015,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="36">
+      <c r="A18" s="30">
         <v>6</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -10023,7 +10023,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="30" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -10031,7 +10031,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="30" t="s">
         <v>82</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -10039,7 +10039,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -10047,7 +10047,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="30" t="s">
         <v>206</v>
       </c>
       <c r="B22" s="1" t="s">
@@ -10055,7 +10055,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="30" t="s">
         <v>208</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -10063,7 +10063,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="30" t="s">
         <v>242</v>
       </c>
       <c r="B24" s="1" t="s">
@@ -10071,7 +10071,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="36">
+      <c r="A25" s="30">
         <v>9</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -10079,18 +10079,18 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="35">
+      <c r="A26" s="29">
         <v>10</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="29" t="s">
         <v>1320</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="35">
+      <c r="A27" s="29">
         <v>11</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="29" t="s">
         <v>1321</v>
       </c>
     </row>
@@ -10474,7 +10474,7 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:IV65536"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10734,7 +10734,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="37" t="s">
         <v>1579</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -10742,7 +10742,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="43" t="s">
+      <c r="A14" s="37" t="s">
         <v>1580</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -10750,7 +10750,7 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="37" t="s">
         <v>1581</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -10770,129 +10770,129 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55" style="30" customWidth="1"/>
-    <col min="4" max="16384" width="11.42578125" style="30"/>
+    <col min="1" max="1" width="19.85546875" style="40" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55" style="40" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="40"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="39" t="s">
         <v>1282</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="41" t="s">
         <v>1258</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="39" t="s">
         <v>1282</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="42" t="s">
         <v>1455</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="38" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="41" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="31" t="s">
+      <c r="B6" s="41" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="31"/>
+      <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="42" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="42" t="s">
         <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="41" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="28"/>
-      <c r="B11" s="31"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="41"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="40" t="s">
         <v>1188</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="43" t="s">
         <v>1259</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="40" t="s">
         <v>1262</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="40" t="s">
         <v>1263</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="33" t="s">
+      <c r="A14" s="43" t="s">
         <v>1260</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="40" t="s">
         <v>1261</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="40" t="s">
         <v>1264</v>
       </c>
     </row>
@@ -14113,7 +14113,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+    <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -14333,7 +14333,7 @@
       <c r="A28" s="23" t="s">
         <v>1426</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="31" t="s">
         <v>1438</v>
       </c>
     </row>
@@ -14341,7 +14341,7 @@
       <c r="A29" s="23" t="s">
         <v>1427</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="31" t="s">
         <v>1439</v>
       </c>
     </row>
@@ -14422,7 +14422,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="32" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -14430,7 +14430,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -14438,7 +14438,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="32" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -14446,7 +14446,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="32" t="s">
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -14454,7 +14454,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -14462,7 +14462,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -14470,13 +14470,13 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="32" t="s">
         <v>28</v>
       </c>
       <c r="B7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="32" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -14484,7 +14484,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="32" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -14492,7 +14492,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="32" t="s">
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -14500,722 +14500,722 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="39" t="s">
+      <c r="A12" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="34" t="s">
         <v>1458</v>
       </c>
-      <c r="C12" s="39" t="s">
+      <c r="C12" s="33" t="s">
         <v>1188</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="35" t="s">
         <v>1195</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="35" t="s">
         <v>1459</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="35" t="s">
         <v>1460</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="35" t="s">
         <v>1196</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="35" t="s">
         <v>1462</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="35" t="s">
         <v>1463</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+    <row r="15" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="35" t="s">
         <v>1197</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="35" t="s">
         <v>1464</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+    <row r="16" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="35" t="s">
         <v>1198</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="35" t="s">
         <v>1465</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="35" t="s">
         <v>1466</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="35" t="s">
         <v>1199</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="35" t="s">
         <v>1461</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="35" t="s">
         <v>1200</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="35" t="s">
         <v>1461</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="35" t="s">
         <v>1461</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+      <c r="A19" s="36" t="s">
         <v>1201</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="36" t="s">
         <v>1467</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="36" t="s">
         <v>1468</v>
       </c>
-      <c r="D19" s="42"/>
+      <c r="D19" s="36"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="36" t="s">
         <v>1202</v>
       </c>
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="36" t="s">
         <v>1469</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="36" t="s">
         <v>1470</v>
       </c>
-      <c r="D20" s="42"/>
-    </row>
-    <row r="21" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+      <c r="D20" s="36"/>
+    </row>
+    <row r="21" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="35" t="s">
         <v>1203</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="35" t="s">
         <v>1471</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="35" t="s">
         <v>1472</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="41" t="s">
+    <row r="22" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="35" t="s">
         <v>1204</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="35" t="s">
         <v>1473</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="35" t="s">
         <v>1474</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="41" t="s">
+    <row r="23" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="35" t="s">
         <v>1205</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="35" t="s">
         <v>1475</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="35" t="s">
         <v>1476</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
+      <c r="A24" s="36" t="s">
         <v>1206</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="36" t="s">
         <v>1477</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="36" t="s">
         <v>1478</v>
       </c>
-      <c r="D24" s="42"/>
+      <c r="D24" s="36"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="42" t="s">
+      <c r="A25" s="36" t="s">
         <v>1207</v>
       </c>
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="36" t="s">
         <v>1479</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="36" t="s">
         <v>1480</v>
       </c>
-      <c r="D25" s="42"/>
+      <c r="D25" s="36"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+      <c r="A26" s="36" t="s">
         <v>1208</v>
       </c>
-      <c r="B26" s="42" t="s">
+      <c r="B26" s="36" t="s">
         <v>1481</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="36" t="s">
         <v>1482</v>
       </c>
-      <c r="D26" s="42"/>
+      <c r="D26" s="36"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>1209</v>
       </c>
-      <c r="B27" s="42" t="s">
+      <c r="B27" s="36" t="s">
         <v>1483</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="36" t="s">
         <v>1484</v>
       </c>
-      <c r="D27" s="42"/>
+      <c r="D27" s="36"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>1210</v>
       </c>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="36" t="s">
         <v>1485</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="36" t="s">
         <v>1486</v>
       </c>
-      <c r="D28" s="42"/>
+      <c r="D28" s="36"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="42" t="s">
+      <c r="A29" s="36" t="s">
         <v>1211</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="36" t="s">
         <v>1487</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-    </row>
-    <row r="30" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41" t="s">
+      <c r="C29" s="36"/>
+      <c r="D29" s="36"/>
+    </row>
+    <row r="30" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="35" t="s">
         <v>1212</v>
       </c>
-      <c r="B30" s="41" t="s">
+      <c r="B30" s="35" t="s">
         <v>1488</v>
       </c>
     </row>
-    <row r="31" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="41" t="s">
+    <row r="31" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="35" t="s">
         <v>1213</v>
       </c>
-      <c r="B31" s="41" t="s">
+      <c r="B31" s="35" t="s">
         <v>1489</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="35" t="s">
         <v>1490</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
+      <c r="A32" s="36" t="s">
         <v>1214</v>
       </c>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="36" t="s">
         <v>1491</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="36" t="s">
         <v>1492</v>
       </c>
-      <c r="D32" s="42"/>
+      <c r="D32" s="36"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="42" t="s">
+      <c r="A33" s="36" t="s">
         <v>1215</v>
       </c>
-      <c r="B33" s="42" t="s">
+      <c r="B33" s="36" t="s">
         <v>1493</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="36" t="s">
         <v>1494</v>
       </c>
-      <c r="D33" s="42"/>
+      <c r="D33" s="36"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="42" t="s">
+      <c r="A34" s="36" t="s">
         <v>1216</v>
       </c>
-      <c r="B34" s="42" t="s">
+      <c r="B34" s="36" t="s">
         <v>1495</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="36" t="s">
         <v>1496</v>
       </c>
-      <c r="D34" s="42"/>
+      <c r="D34" s="36"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="36" t="s">
         <v>1217</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="36" t="s">
         <v>1497</v>
       </c>
-      <c r="C35" s="42" t="s">
+      <c r="C35" s="36" t="s">
         <v>1498</v>
       </c>
-      <c r="D35" s="42"/>
-    </row>
-    <row r="36" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+      <c r="D35" s="36"/>
+    </row>
+    <row r="36" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="35" t="s">
         <v>1218</v>
       </c>
-      <c r="B36" s="41" t="s">
+      <c r="B36" s="35" t="s">
         <v>1499</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="35" t="s">
         <v>1500</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="41" t="s">
+    <row r="37" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="35" t="s">
         <v>1219</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="35" t="s">
         <v>1501</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="35" t="s">
         <v>1502</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="42" t="s">
+      <c r="A38" s="36" t="s">
         <v>1220</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="36" t="s">
         <v>1503</v>
       </c>
-      <c r="C38" s="42" t="s">
+      <c r="C38" s="36" t="s">
         <v>1504</v>
       </c>
-      <c r="D38" s="42"/>
+      <c r="D38" s="36"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="42" t="s">
+      <c r="A39" s="36" t="s">
         <v>1221</v>
       </c>
-      <c r="B39" s="42" t="s">
+      <c r="B39" s="36" t="s">
         <v>1505</v>
       </c>
-      <c r="C39" s="42" t="s">
+      <c r="C39" s="36" t="s">
         <v>1506</v>
       </c>
-      <c r="D39" s="42"/>
+      <c r="D39" s="36"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="42" t="s">
+      <c r="A40" s="36" t="s">
         <v>1222</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B40" s="36" t="s">
         <v>1507</v>
       </c>
-      <c r="C40" s="42" t="s">
+      <c r="C40" s="36" t="s">
         <v>1506</v>
       </c>
-      <c r="D40" s="42"/>
-    </row>
-    <row r="41" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="41" t="s">
+      <c r="D40" s="36"/>
+    </row>
+    <row r="41" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="35" t="s">
         <v>1223</v>
       </c>
-      <c r="B41" s="41" t="s">
+      <c r="B41" s="35" t="s">
         <v>1508</v>
       </c>
-      <c r="C41" s="41" t="s">
+      <c r="C41" s="35" t="s">
         <v>1509</v>
       </c>
     </row>
-    <row r="42" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="41" t="s">
+    <row r="42" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="35" t="s">
         <v>1224</v>
       </c>
-      <c r="B42" s="41" t="s">
+      <c r="B42" s="35" t="s">
         <v>1510</v>
       </c>
-      <c r="C42" s="41" t="s">
+      <c r="C42" s="35" t="s">
         <v>1511</v>
       </c>
     </row>
-    <row r="43" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="41" t="s">
+    <row r="43" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="35" t="s">
         <v>1225</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="35" t="s">
         <v>1512</v>
       </c>
-      <c r="C43" s="41" t="s">
+      <c r="C43" s="35" t="s">
         <v>1513</v>
       </c>
     </row>
-    <row r="44" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="41" t="s">
+    <row r="44" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="35" t="s">
         <v>1226</v>
       </c>
-      <c r="B44" s="41" t="s">
+      <c r="B44" s="35" t="s">
         <v>1514</v>
       </c>
-      <c r="C44" s="41" t="s">
+      <c r="C44" s="35" t="s">
         <v>1515</v>
       </c>
     </row>
-    <row r="45" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="41" t="s">
+    <row r="45" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="35" t="s">
         <v>1227</v>
       </c>
-      <c r="B45" s="41" t="s">
+      <c r="B45" s="35" t="s">
         <v>1516</v>
       </c>
-      <c r="C45" s="41" t="s">
+      <c r="C45" s="35" t="s">
         <v>1517</v>
       </c>
     </row>
-    <row r="46" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="41" t="s">
+    <row r="46" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="35" t="s">
         <v>1228</v>
       </c>
-      <c r="B46" s="41" t="s">
+      <c r="B46" s="35" t="s">
         <v>1518</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="41" t="s">
+    <row r="47" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="35" t="s">
         <v>1247</v>
       </c>
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="35" t="s">
         <v>1519</v>
       </c>
-      <c r="C47" s="41" t="s">
+      <c r="C47" s="35" t="s">
         <v>1520</v>
       </c>
     </row>
-    <row r="48" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="41" t="s">
+    <row r="48" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="35" t="s">
         <v>1229</v>
       </c>
-      <c r="B48" s="41" t="s">
+      <c r="B48" s="35" t="s">
         <v>1521</v>
       </c>
-      <c r="C48" s="41" t="s">
+      <c r="C48" s="35" t="s">
         <v>1522</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="42" t="s">
+      <c r="A49" s="36" t="s">
         <v>1230</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B49" s="36" t="s">
         <v>1523</v>
       </c>
-      <c r="C49" s="42" t="s">
+      <c r="C49" s="36" t="s">
         <v>1524</v>
       </c>
-      <c r="D49" s="42"/>
+      <c r="D49" s="36"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="36" t="s">
         <v>1231</v>
       </c>
-      <c r="B50" s="42" t="s">
+      <c r="B50" s="36" t="s">
         <v>1525</v>
       </c>
-      <c r="C50" s="42" t="s">
+      <c r="C50" s="36" t="s">
         <v>1526</v>
       </c>
-      <c r="D50" s="42"/>
+      <c r="D50" s="36"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" s="42" t="s">
+      <c r="A51" s="36" t="s">
         <v>1232</v>
       </c>
-      <c r="B51" s="42" t="s">
+      <c r="B51" s="36" t="s">
         <v>1527</v>
       </c>
-      <c r="C51" s="42" t="s">
+      <c r="C51" s="36" t="s">
         <v>1528</v>
       </c>
-      <c r="D51" s="42"/>
-    </row>
-    <row r="52" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="41" t="s">
+      <c r="D51" s="36"/>
+    </row>
+    <row r="52" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="35" t="s">
         <v>1233</v>
       </c>
-      <c r="B52" s="41" t="s">
+      <c r="B52" s="35" t="s">
         <v>1529</v>
       </c>
-      <c r="C52" s="41" t="s">
+      <c r="C52" s="35" t="s">
         <v>1530</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="41" t="s">
+    <row r="53" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="35" t="s">
         <v>1234</v>
       </c>
-      <c r="B53" s="41" t="s">
+      <c r="B53" s="35" t="s">
         <v>1531</v>
       </c>
-      <c r="C53" s="41" t="s">
+      <c r="C53" s="35" t="s">
         <v>1532</v>
       </c>
     </row>
-    <row r="54" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="41" t="s">
+    <row r="54" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="35" t="s">
         <v>1235</v>
       </c>
-      <c r="B54" s="41" t="s">
+      <c r="B54" s="35" t="s">
         <v>1533</v>
       </c>
-      <c r="C54" s="41" t="s">
+      <c r="C54" s="35" t="s">
         <v>1534</v>
       </c>
     </row>
-    <row r="55" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="41" t="s">
+    <row r="55" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="35" t="s">
         <v>1535</v>
       </c>
-      <c r="B55" s="41" t="s">
+      <c r="B55" s="35" t="s">
         <v>1536</v>
       </c>
-      <c r="C55" s="41" t="s">
+      <c r="C55" s="35" t="s">
         <v>1537</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="41" t="s">
+    <row r="56" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="35" t="s">
         <v>1236</v>
       </c>
-      <c r="B56" s="41" t="s">
+      <c r="B56" s="35" t="s">
         <v>1538</v>
       </c>
-      <c r="C56" s="41" t="s">
+      <c r="C56" s="35" t="s">
         <v>1539</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="41" t="s">
+    <row r="57" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="35" t="s">
         <v>1248</v>
       </c>
-      <c r="B57" s="41" t="s">
+      <c r="B57" s="35" t="s">
         <v>1540</v>
       </c>
-      <c r="C57" s="41" t="s">
+      <c r="C57" s="35" t="s">
         <v>1541</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="41" t="s">
+    <row r="58" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="35" t="s">
         <v>1542</v>
       </c>
-      <c r="B58" s="41" t="s">
+      <c r="B58" s="35" t="s">
         <v>1543</v>
       </c>
-      <c r="C58" s="41" t="s">
+      <c r="C58" s="35" t="s">
         <v>1544</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="41" t="s">
+    <row r="59" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="35" t="s">
         <v>1237</v>
       </c>
-      <c r="B59" s="41" t="s">
+      <c r="B59" s="35" t="s">
         <v>1545</v>
       </c>
-      <c r="C59" s="41" t="s">
+      <c r="C59" s="35" t="s">
         <v>1546</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="41" t="s">
+    <row r="60" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="35" t="s">
         <v>1239</v>
       </c>
-      <c r="B60" s="41" t="s">
+      <c r="B60" s="35" t="s">
         <v>1547</v>
       </c>
-      <c r="C60" s="41" t="s">
+      <c r="C60" s="35" t="s">
         <v>1548</v>
       </c>
     </row>
-    <row r="61" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="41" t="s">
+    <row r="61" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="35" t="s">
         <v>1240</v>
       </c>
-      <c r="B61" s="41" t="s">
+      <c r="B61" s="35" t="s">
         <v>1549</v>
       </c>
-      <c r="C61" s="41" t="s">
+      <c r="C61" s="35" t="s">
         <v>1550</v>
       </c>
     </row>
-    <row r="62" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="41" t="s">
+    <row r="62" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="35" t="s">
         <v>1238</v>
       </c>
-      <c r="B62" s="41" t="s">
+      <c r="B62" s="35" t="s">
         <v>1551</v>
       </c>
-      <c r="C62" s="41" t="s">
+      <c r="C62" s="35" t="s">
         <v>1552</v>
       </c>
     </row>
-    <row r="63" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="41" t="s">
+    <row r="63" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="35" t="s">
         <v>1241</v>
       </c>
-      <c r="B63" s="41" t="s">
+      <c r="B63" s="35" t="s">
         <v>1553</v>
       </c>
-      <c r="C63" s="41" t="s">
+      <c r="C63" s="35" t="s">
         <v>1554</v>
       </c>
     </row>
-    <row r="64" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="41" t="s">
+    <row r="64" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="35" t="s">
         <v>1242</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="35" t="s">
         <v>1555</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C64" s="35" t="s">
         <v>1556</v>
       </c>
     </row>
-    <row r="65" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="41" t="s">
+    <row r="65" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="35" t="s">
         <v>1243</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="35" t="s">
         <v>1557</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="C65" s="35" t="s">
         <v>1558</v>
       </c>
     </row>
-    <row r="66" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="41" t="s">
+    <row r="66" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="35" t="s">
         <v>1244</v>
       </c>
-      <c r="B66" s="41" t="s">
+      <c r="B66" s="35" t="s">
         <v>1559</v>
       </c>
-      <c r="C66" s="41" t="s">
+      <c r="C66" s="35" t="s">
         <v>1560</v>
       </c>
     </row>
-    <row r="67" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="41" t="s">
+    <row r="67" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="35" t="s">
         <v>1245</v>
       </c>
-      <c r="B67" s="41" t="s">
+      <c r="B67" s="35" t="s">
         <v>1561</v>
       </c>
-      <c r="C67" s="41" t="s">
+      <c r="C67" s="35" t="s">
         <v>1562</v>
       </c>
     </row>
-    <row r="68" spans="1:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="41" t="s">
+    <row r="68" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="35" t="s">
         <v>1246</v>
       </c>
-      <c r="B68" s="41" t="s">
+      <c r="B68" s="35" t="s">
         <v>1563</v>
       </c>
-      <c r="C68" s="41" t="s">
+      <c r="C68" s="35" t="s">
         <v>1564</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="42" t="s">
+      <c r="A69" s="36" t="s">
         <v>1189</v>
       </c>
-      <c r="B69" s="42" t="s">
+      <c r="B69" s="36" t="s">
         <v>1565</v>
       </c>
-      <c r="C69" s="42" t="s">
+      <c r="C69" s="36" t="s">
         <v>1566</v>
       </c>
-      <c r="D69" s="42"/>
+      <c r="D69" s="36"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="42" t="s">
+      <c r="A70" s="36" t="s">
         <v>1190</v>
       </c>
-      <c r="B70" s="42" t="s">
+      <c r="B70" s="36" t="s">
         <v>1567</v>
       </c>
-      <c r="C70" s="42" t="s">
+      <c r="C70" s="36" t="s">
         <v>1568</v>
       </c>
-      <c r="D70" s="42"/>
+      <c r="D70" s="36"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="42" t="s">
+      <c r="A71" s="36" t="s">
         <v>1191</v>
       </c>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="36" t="s">
         <v>1569</v>
       </c>
-      <c r="C71" s="42" t="s">
+      <c r="C71" s="36" t="s">
         <v>1570</v>
       </c>
-      <c r="D71" s="42"/>
+      <c r="D71" s="36"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="42" t="s">
+      <c r="A72" s="36" t="s">
         <v>1192</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="36" t="s">
         <v>1571</v>
       </c>
-      <c r="C72" s="42" t="s">
+      <c r="C72" s="36" t="s">
         <v>1572</v>
       </c>
-      <c r="D72" s="42"/>
+      <c r="D72" s="36"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="42" t="s">
+      <c r="A73" s="36" t="s">
         <v>1193</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="36" t="s">
         <v>1573</v>
       </c>
-      <c r="C73" s="42" t="s">
+      <c r="C73" s="36" t="s">
         <v>1574</v>
       </c>
-      <c r="D73" s="42"/>
+      <c r="D73" s="36"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="42" t="s">
+      <c r="A74" s="36" t="s">
         <v>1194</v>
       </c>
-      <c r="B74" s="42" t="s">
+      <c r="B74" s="36" t="s">
         <v>1575</v>
       </c>
-      <c r="C74" s="42" t="s">
+      <c r="C74" s="36" t="s">
         <v>1576</v>
       </c>
-      <c r="D74" s="42"/>
+      <c r="D74" s="36"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20170903T1214 - EO Expected Elements
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -18,20 +18,21 @@
     <sheet name="CurrencyCode" sheetId="191" r:id="rId9"/>
     <sheet name="DocRefContentType" sheetId="192" r:id="rId10"/>
     <sheet name="EOIDType" sheetId="198" r:id="rId11"/>
-    <sheet name="EORoleType" sheetId="152" r:id="rId12"/>
-    <sheet name="EULanguageCode" sheetId="145" r:id="rId13"/>
-    <sheet name="FinancialRatioType" sheetId="200" r:id="rId14"/>
-    <sheet name="EvaluationMethodType" sheetId="197" r:id="rId15"/>
-    <sheet name="LegislationType" sheetId="175" r:id="rId16"/>
-    <sheet name="NumberOfLotsCode" sheetId="196" r:id="rId17"/>
-    <sheet name="PeriodMeasureType" sheetId="189" r:id="rId18"/>
-    <sheet name="ProcedureType" sheetId="146" r:id="rId19"/>
-    <sheet name="ProfileExecutionID" sheetId="161" r:id="rId20"/>
-    <sheet name="ProjectType" sheetId="147" r:id="rId21"/>
-    <sheet name="PropertyGroupType" sheetId="203" r:id="rId22"/>
-    <sheet name="QualificationApplicationType" sheetId="195" r:id="rId23"/>
-    <sheet name="ServicesProjectSubType" sheetId="158" r:id="rId24"/>
-    <sheet name="TechnicalCapabilityType" sheetId="149" r:id="rId25"/>
+    <sheet name="EOIndustryClassificationCode" sheetId="204" r:id="rId12"/>
+    <sheet name="EORoleType" sheetId="152" r:id="rId13"/>
+    <sheet name="EULanguageCode" sheetId="145" r:id="rId14"/>
+    <sheet name="FinancialRatioType" sheetId="200" r:id="rId15"/>
+    <sheet name="EvaluationMethodType" sheetId="197" r:id="rId16"/>
+    <sheet name="LegislationType" sheetId="175" r:id="rId17"/>
+    <sheet name="NumberOfLotsCode" sheetId="196" r:id="rId18"/>
+    <sheet name="PeriodMeasureType" sheetId="189" r:id="rId19"/>
+    <sheet name="ProcedureType" sheetId="146" r:id="rId20"/>
+    <sheet name="ProfileExecutionID" sheetId="161" r:id="rId21"/>
+    <sheet name="ProjectType" sheetId="147" r:id="rId22"/>
+    <sheet name="PropertyGroupType" sheetId="203" r:id="rId23"/>
+    <sheet name="QualificationApplicationType" sheetId="195" r:id="rId24"/>
+    <sheet name="ServicesProjectSubType" sheetId="158" r:id="rId25"/>
+    <sheet name="TechnicalCapabilityType" sheetId="149" r:id="rId26"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="7">CriteriaType!$A$1:$C$75</definedName>
@@ -280,7 +281,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2205" uniqueCount="1588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="1600">
   <si>
     <t>SV</t>
   </si>
@@ -5045,13 +5046,49 @@
   </si>
   <si>
     <t>Points at the instance of an evidence</t>
+  </si>
+  <si>
+    <t>EOIndustryClassificationCode</t>
+  </si>
+  <si>
+    <t>Economic Operator Industry Classification Code</t>
+  </si>
+  <si>
+    <t>MICRO</t>
+  </si>
+  <si>
+    <t>SMALL</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>LARGE</t>
+  </si>
+  <si>
+    <t>Micro Enterprise</t>
+  </si>
+  <si>
+    <t>Small Enterprise</t>
+  </si>
+  <si>
+    <t>Medium Enterprise</t>
+  </si>
+  <si>
+    <t>Non SME, Large Company</t>
+  </si>
+  <si>
+    <t>SME</t>
+  </si>
+  <si>
+    <t>Small or Medium Enterprise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -5141,6 +5178,16 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -5242,7 +5289,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5333,6 +5380,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Nor_x0004_al" xfId="1"/>
@@ -5340,7 +5389,7 @@
     <cellStyle name="Normal 2 2" xfId="2"/>
     <cellStyle name="Normal 2 3" xfId="3"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="36">
     <dxf>
       <font>
         <b val="0"/>
@@ -5646,6 +5695,23 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9.5"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -6678,10 +6744,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7837" name="Table7837" displayName="Table7837" ref="A12:B35" tableType="xml" totalsRowShown="0" connectionId="66">
   <autoFilter ref="A12:B35"/>
   <tableColumns count="2">
-    <tableColumn id="1" uniqueName="Code" name="Code" dataDxfId="34">
+    <tableColumn id="1" uniqueName="Code" name="Code" dataDxfId="35">
       <xmlColumnPr mapId="614" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="33">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="34">
       <xmlColumnPr mapId="614" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6690,6 +6756,21 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table78042" displayName="Table78042" ref="A12:B17" tableType="xml" totalsRowShown="0" connectionId="77">
+  <autoFilter ref="A12:B17"/>
+  <tableColumns count="2">
+    <tableColumn id="1" uniqueName="Code" name="Code">
+      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="24">
+      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7804" name="Table7804" displayName="Table7804" ref="A12:C16" tableType="xml" totalsRowShown="0" connectionId="77">
   <autoFilter ref="A12:C16"/>
   <tableColumns count="3">
@@ -6705,7 +6786,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7606" name="Table7606" displayName="Table7606" ref="A12:B36" tableType="xml" totalsRowShown="0" connectionId="64">
   <autoFilter ref="A12:B36"/>
   <tableColumns count="2">
@@ -6720,7 +6801,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24511" name="Table783724512" displayName="Table783724512" ref="A12:C41" tableType="xml" totalsRowShown="0" connectionId="66">
   <autoFilter ref="A12:C41"/>
   <tableColumns count="3">
@@ -6736,7 +6817,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24096" name="Table783713621145522280724097" displayName="Table783713621145522280724097" ref="A12:B14" totalsRowShown="0">
   <autoFilter ref="A12:B14"/>
   <sortState ref="A13:B41">
@@ -6750,7 +6831,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22806" name="Table7837136211455222807" displayName="Table7837136211455222807" ref="A12:B17" totalsRowShown="0">
   <autoFilter ref="A12:B17"/>
   <sortState ref="A13:B41">
@@ -6764,7 +6845,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24095" name="Table760624096" displayName="Table760624096" ref="A12:C15" tableType="xml" totalsRowShown="0" connectionId="64">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
@@ -6780,7 +6861,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22400" name="Table783713621145522170522099221992230022401" displayName="Table783713621145522170522099221992230022401" ref="A12:B14" tableType="xml" totalsRowShown="0" connectionId="66">
   <autoFilter ref="A12:B14"/>
   <sortState ref="A13:B41">
@@ -6798,7 +6879,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7627" name="Table7627" displayName="Table7627" ref="A12:B27" tableType="xml" totalsRowShown="0" connectionId="61">
   <autoFilter ref="A12:B27"/>
   <tableColumns count="2">
@@ -6813,7 +6894,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10009" name="Table762710010" displayName="Table762710010" ref="A12:B16" tableType="xml" totalsRowShown="0" connectionId="62">
   <autoFilter ref="A12:B16"/>
   <tableColumns count="2">
@@ -6828,7 +6909,18 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16245" name="Table783716246" displayName="Table783716246" ref="A12:B18" totalsRowShown="0">
+  <autoFilter ref="A12:B18"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Code" dataDxfId="33"/>
+    <tableColumn id="2" name="Value" dataDxfId="32"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7638" name="Table7638" displayName="Table7638" ref="A12:B19" tableType="xml" totalsRowShown="0" connectionId="72">
   <autoFilter ref="A12:B19"/>
   <tableColumns count="2">
@@ -6843,18 +6935,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="16245" name="Table783716246" displayName="Table783716246" ref="A12:B18" totalsRowShown="0">
-  <autoFilter ref="A12:B18"/>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="32"/>
-    <tableColumn id="2" name="Value" dataDxfId="31"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26629" name="Table763826630" displayName="Table763826630" ref="A12:B15" tableType="xml" totalsRowShown="0" connectionId="72">
   <autoFilter ref="A12:B15"/>
   <tableColumns count="2">
@@ -6869,7 +6950,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23994" name="Table763823995" displayName="Table763823995" ref="A12:C14" tableType="xml" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" connectionId="72">
   <autoFilter ref="A12:C14"/>
   <tableColumns count="3">
@@ -6885,7 +6966,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7870" name="Table7870" displayName="Table7870" ref="A12:B39" tableType="xml" totalsRowShown="0" connectionId="69">
   <autoFilter ref="A12:B39"/>
   <tableColumns count="2">
@@ -6900,7 +6981,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table24.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7763" name="Table7763" displayName="Table7763" ref="A12:B30" tableType="xml" totalsRowShown="0" connectionId="74">
   <autoFilter ref="A12:B30"/>
   <tableColumns count="2">
@@ -6922,7 +7003,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="30">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="31">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6937,7 +7018,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="29">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="30">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6952,7 +7033,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="28">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="29">
       <xmlColumnPr mapId="603" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -6967,8 +7048,8 @@
     <sortCondition ref="A13"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="27"/>
-    <tableColumn id="2" name="Value" dataDxfId="26"/>
+    <tableColumn id="1" name="Code" dataDxfId="28"/>
+    <tableColumn id="2" name="Value" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6990,7 +7071,7 @@
   <autoFilter ref="A12:B32"/>
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
-    <tableColumn id="2" name="Value" dataDxfId="25"/>
+    <tableColumn id="2" name="Value" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7003,7 +7084,7 @@
     <tableColumn id="1" uniqueName="Code" name="Code">
       <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="24">
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="25">
       <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7763,7 +7844,7 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8461,11 +8542,158 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1589</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1588</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>1590</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>1591</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>1592</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>1596</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="45" t="s">
+        <v>1598</v>
+      </c>
+      <c r="B16" s="44" t="s">
+        <v>1599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>1593</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>1597</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView zoomScaleNormal="115" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8616,7 +8844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B36"/>
@@ -8909,7 +9137,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
@@ -9338,7 +9566,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -9462,7 +9690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -9609,7 +9837,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -9751,7 +9979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -9873,232 +10101,6 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="30">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="30">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="30">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="30">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="29">
-        <v>10</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
-        <v>11</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -10335,6 +10337,232 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="30">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="30">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="30">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="30">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="30">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="30">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>10</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>11</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -10468,7 +10696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B19"/>
@@ -10633,7 +10861,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -10765,7 +10993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -10905,7 +11133,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15">
     <tabColor theme="0" tint="-0.249977111117893"/>
@@ -11225,7 +11453,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:B39"/>

</xml_diff>

<commit_message>
20170903T2059 - EO Data Structures and XML example (1/2)
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -13,29 +13,29 @@
     <sheet name="ContractType" sheetId="144" r:id="rId4"/>
     <sheet name="CountryCodeIdentifier" sheetId="190" r:id="rId5"/>
     <sheet name="CriterionElementType" sheetId="202" r:id="rId6"/>
-    <sheet name="ResponseDataType" sheetId="185" r:id="rId7"/>
-    <sheet name="CriteriaType" sheetId="193" r:id="rId8"/>
-    <sheet name="CurrencyCode" sheetId="191" r:id="rId9"/>
-    <sheet name="DocRefContentType" sheetId="192" r:id="rId10"/>
-    <sheet name="EOIDType" sheetId="198" r:id="rId11"/>
-    <sheet name="EOIndustryClassificationCode" sheetId="204" r:id="rId12"/>
-    <sheet name="EORoleType" sheetId="152" r:id="rId13"/>
-    <sheet name="EULanguageCode" sheetId="145" r:id="rId14"/>
-    <sheet name="FinancialRatioType" sheetId="200" r:id="rId15"/>
-    <sheet name="EvaluationMethodType" sheetId="197" r:id="rId16"/>
-    <sheet name="LegislationType" sheetId="175" r:id="rId17"/>
-    <sheet name="NumberOfLotsCode" sheetId="196" r:id="rId18"/>
-    <sheet name="PeriodMeasureType" sheetId="189" r:id="rId19"/>
-    <sheet name="ProcedureType" sheetId="146" r:id="rId20"/>
-    <sheet name="ProfileExecutionID" sheetId="161" r:id="rId21"/>
-    <sheet name="ProjectType" sheetId="147" r:id="rId22"/>
-    <sheet name="PropertyGroupType" sheetId="203" r:id="rId23"/>
-    <sheet name="QualificationApplicationType" sheetId="195" r:id="rId24"/>
+    <sheet name="CriteriaType" sheetId="193" r:id="rId7"/>
+    <sheet name="CurrencyCode" sheetId="191" r:id="rId8"/>
+    <sheet name="DocRefContentType" sheetId="192" r:id="rId9"/>
+    <sheet name="EOIDType" sheetId="198" r:id="rId10"/>
+    <sheet name="EOIndustryClassificationCode" sheetId="204" r:id="rId11"/>
+    <sheet name="EORoleType" sheetId="152" r:id="rId12"/>
+    <sheet name="EULanguageCode" sheetId="145" r:id="rId13"/>
+    <sheet name="FinancialRatioType" sheetId="200" r:id="rId14"/>
+    <sheet name="EvaluationMethodType" sheetId="197" r:id="rId15"/>
+    <sheet name="LegislationType" sheetId="175" r:id="rId16"/>
+    <sheet name="NumberOfLotsCode" sheetId="196" r:id="rId17"/>
+    <sheet name="PeriodMeasureType" sheetId="189" r:id="rId18"/>
+    <sheet name="ProcedureType" sheetId="146" r:id="rId19"/>
+    <sheet name="ProfileExecutionID" sheetId="161" r:id="rId20"/>
+    <sheet name="ProjectType" sheetId="147" r:id="rId21"/>
+    <sheet name="PropertyGroupType" sheetId="203" r:id="rId22"/>
+    <sheet name="QualificationApplicationType" sheetId="195" r:id="rId23"/>
+    <sheet name="ResponseDataType" sheetId="185" r:id="rId24"/>
     <sheet name="ServicesProjectSubType" sheetId="158" r:id="rId25"/>
     <sheet name="TechnicalCapabilityType" sheetId="149" r:id="rId26"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">CriteriaType!$A$1:$C$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">CriteriaType!$A$1:$C$75</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -5186,6 +5186,7 @@
       <name val="Arial"/>
     </font>
     <font>
+      <b/>
       <u/>
       <sz val="10"/>
       <name val="Arial"/>
@@ -6756,21 +6757,6 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table78042" displayName="Table78042" ref="A12:B17" tableType="xml" totalsRowShown="0" connectionId="77">
-  <autoFilter ref="A12:B17"/>
-  <tableColumns count="2">
-    <tableColumn id="1" uniqueName="Code" name="Code">
-      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="24">
-      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7804" name="Table7804" displayName="Table7804" ref="A12:C16" tableType="xml" totalsRowShown="0" connectionId="77">
   <autoFilter ref="A12:C16"/>
   <tableColumns count="3">
@@ -6786,7 +6772,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7606" name="Table7606" displayName="Table7606" ref="A12:B36" tableType="xml" totalsRowShown="0" connectionId="64">
   <autoFilter ref="A12:B36"/>
   <tableColumns count="2">
@@ -6801,7 +6787,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24511" name="Table783724512" displayName="Table783724512" ref="A12:C41" tableType="xml" totalsRowShown="0" connectionId="66">
   <autoFilter ref="A12:C41"/>
   <tableColumns count="3">
@@ -6817,7 +6803,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24096" name="Table783713621145522280724097" displayName="Table783713621145522280724097" ref="A12:B14" totalsRowShown="0">
   <autoFilter ref="A12:B14"/>
   <sortState ref="A13:B41">
@@ -6831,7 +6817,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22806" name="Table7837136211455222807" displayName="Table7837136211455222807" ref="A12:B17" totalsRowShown="0">
   <autoFilter ref="A12:B17"/>
   <sortState ref="A13:B41">
@@ -6845,7 +6831,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24095" name="Table760624096" displayName="Table760624096" ref="A12:C15" tableType="xml" totalsRowShown="0" connectionId="64">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
@@ -6861,7 +6847,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22400" name="Table783713621145522170522099221992230022401" displayName="Table783713621145522170522099221992230022401" ref="A12:B14" tableType="xml" totalsRowShown="0" connectionId="66">
   <autoFilter ref="A12:B14"/>
   <sortState ref="A13:B41">
@@ -6879,7 +6865,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7627" name="Table7627" displayName="Table7627" ref="A12:B27" tableType="xml" totalsRowShown="0" connectionId="61">
   <autoFilter ref="A12:B27"/>
   <tableColumns count="2">
@@ -6894,7 +6880,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10009" name="Table762710010" displayName="Table762710010" ref="A12:B16" tableType="xml" totalsRowShown="0" connectionId="62">
   <autoFilter ref="A12:B16"/>
   <tableColumns count="2">
@@ -6903,6 +6889,21 @@
     </tableColumn>
     <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="11">
       <xmlColumnPr mapId="631" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7638" name="Table7638" displayName="Table7638" ref="A12:B19" tableType="xml" totalsRowShown="0" connectionId="72">
+  <autoFilter ref="A12:B19"/>
+  <tableColumns count="2">
+    <tableColumn id="1" uniqueName="Code" name="Code" dataDxfId="10">
+      <xmlColumnPr mapId="606" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Value" name="Value">
+      <xmlColumnPr mapId="606" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6921,21 +6922,6 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7638" name="Table7638" displayName="Table7638" ref="A12:B19" tableType="xml" totalsRowShown="0" connectionId="72">
-  <autoFilter ref="A12:B19"/>
-  <tableColumns count="2">
-    <tableColumn id="1" uniqueName="Code" name="Code" dataDxfId="10">
-      <xmlColumnPr mapId="606" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Value" name="Value">
-      <xmlColumnPr mapId="606" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
-    </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26629" name="Table763826630" displayName="Table763826630" ref="A12:B15" tableType="xml" totalsRowShown="0" connectionId="72">
   <autoFilter ref="A12:B15"/>
   <tableColumns count="2">
@@ -6950,7 +6936,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23994" name="Table763823995" displayName="Table763823995" ref="A12:C14" tableType="xml" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7" connectionId="72">
   <autoFilter ref="A12:C14"/>
   <tableColumns count="3">
@@ -6961,6 +6947,20 @@
       <xmlColumnPr mapId="606" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
     <tableColumn id="3" uniqueName="3" name="Description" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22805" name="Table783713621145522170522806" displayName="Table783713621145522170522806" ref="A12:B35" totalsRowShown="0">
+  <autoFilter ref="A12:B35"/>
+  <sortState ref="A13:B23">
+    <sortCondition ref="A13"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Code" dataDxfId="28"/>
+    <tableColumn id="2" name="Value" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7042,20 +7042,6 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="22805" name="Table783713621145522170522806" displayName="Table783713621145522170522806" ref="A12:B35" totalsRowShown="0">
-  <autoFilter ref="A12:B35"/>
-  <sortState ref="A13:B23">
-    <sortCondition ref="A13"/>
-  </sortState>
-  <tableColumns count="2">
-    <tableColumn id="1" name="Code" dataDxfId="28"/>
-    <tableColumn id="2" name="Value" dataDxfId="27"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="26628" name="List11_1914365" displayName="List11_1914365" ref="A12:C74" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Code"/>
@@ -7066,7 +7052,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="23205" name="Table75952343623206" displayName="Table75952343623206" ref="A12:B32" totalsRowShown="0">
   <autoFilter ref="A12:B32"/>
   <tableColumns count="2">
@@ -7077,7 +7063,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="24301" name="Table780424302" displayName="Table780424302" ref="A12:B17" tableType="xml" totalsRowShown="0" connectionId="77">
   <autoFilter ref="A12:B17"/>
   <tableColumns count="2">
@@ -7085,6 +7071,21 @@
       <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
     </tableColumn>
     <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="25">
+      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table78042" displayName="Table78042" ref="A12:B17" tableType="xml" totalsRowShown="0" connectionId="77">
+  <autoFilter ref="A12:B17"/>
+  <tableColumns count="2">
+    <tableColumn id="1" uniqueName="Code" name="Code">
+      <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Code" xmlDataType="integer"/>
+    </tableColumn>
+    <tableColumn id="2" uniqueName="Value" name="Value" dataDxfId="24">
       <xmlColumnPr mapId="611" xpath="/CodeList/ValuesSet/ValueSet/Value" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -7844,7 +7845,7 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8126,275 +8127,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B32"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>1176</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>1182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
-        <v>1177</v>
-      </c>
-      <c r="B13" s="12" t="s">
-        <v>1266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
-        <v>1178</v>
-      </c>
-      <c r="B14" s="12" t="s">
-        <v>1179</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="26" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="26" t="s">
-        <v>233</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
-        <v>234</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
-        <v>235</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
-        <v>236</v>
-      </c>
-      <c r="B19" s="12" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>237</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>238</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>84</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>1265</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>1404</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>1411</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>1405</v>
-      </c>
-      <c r="B25" s="12" t="s">
-        <v>1413</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>1406</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>1412</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>1407</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>1410</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>1408</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>1414</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>1409</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>1415</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>1416</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>1417</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>1420</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>1418</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>1421</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -8540,11 +8272,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8553,7 +8285,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="45" t="s">
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -8663,7 +8395,7 @@
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="12" t="s">
         <v>1598</v>
       </c>
       <c r="B16" s="44" t="s">
@@ -8687,7 +8419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
   <dimension ref="A1:C16"/>
@@ -8844,7 +8576,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:B36"/>
@@ -9137,7 +8869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C41"/>
   <sheetViews>
@@ -9566,7 +9298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -9690,7 +9422,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B17"/>
   <sheetViews>
@@ -9837,7 +9569,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -9979,7 +9711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -10101,6 +9833,232 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet12"/>
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="30">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="30">
+        <v>2</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="30">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="30">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="30">
+        <v>6</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="30" t="s">
+        <v>242</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="30">
+        <v>9</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="29">
+        <v>10</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>1320</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="29">
+        <v>11</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -10337,232 +10295,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet12"/>
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="19.7109375" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1"/>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="30">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="30">
-        <v>2</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="30">
-        <v>3</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="30">
-        <v>4</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="30">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="30" t="s">
-        <v>206</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="30" t="s">
-        <v>208</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="30" t="s">
-        <v>242</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="30">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="29">
-        <v>10</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>1320</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="29">
-        <v>11</v>
-      </c>
-      <c r="B27" s="29" t="s">
-        <v>1321</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId3"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:B16"/>
   <sheetViews>
@@ -10696,7 +10428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:B19"/>
@@ -10861,7 +10593,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -10993,7 +10725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
@@ -11122,6 +10854,299 @@
       </c>
       <c r="C14" s="40" t="s">
         <v>1264</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27" style="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="175.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>279</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="23" t="s">
+        <v>1586</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>1587</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="20" t="s">
+        <v>272</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="23" t="s">
+        <v>290</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>292</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="20" t="s">
+        <v>294</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="20" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="20" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>1585</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="20" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>1403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="23" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B28" s="31" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="23" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B29" s="31" t="s">
+        <v>1439</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="23" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>1437</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="23" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>1436</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="23" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B32" s="23" t="s">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="23" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B33" s="23" t="s">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="23" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="23" t="s">
+        <v>1440</v>
+      </c>
+      <c r="B35" s="23" t="s">
+        <v>1441</v>
       </c>
     </row>
   </sheetData>
@@ -11746,7 +11771,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B9"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14339,299 +14364,6 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27" style="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="175.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>1455</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>270</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="20" t="s">
-        <v>279</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>271</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B17" s="20" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
-        <v>1586</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>285</v>
-      </c>
-      <c r="B19" s="20" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="20" t="s">
-        <v>272</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
-        <v>290</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
-        <v>292</v>
-      </c>
-      <c r="B23" s="20" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="B24" s="20" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>1269</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>1270</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="20" t="s">
-        <v>1314</v>
-      </c>
-      <c r="B26" s="20" t="s">
-        <v>1585</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
-        <v>1402</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>1403</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
-        <v>1426</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>1438</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
-        <v>1427</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>1439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
-        <v>1428</v>
-      </c>
-      <c r="B30" s="23" t="s">
-        <v>1437</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
-        <v>1429</v>
-      </c>
-      <c r="B31" s="23" t="s">
-        <v>1436</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
-        <v>1430</v>
-      </c>
-      <c r="B32" s="23" t="s">
-        <v>1435</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
-        <v>1431</v>
-      </c>
-      <c r="B33" s="23" t="s">
-        <v>1433</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
-        <v>1432</v>
-      </c>
-      <c r="B34" s="23" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
-        <v>1440</v>
-      </c>
-      <c r="B35" s="23" t="s">
-        <v>1441</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -15454,7 +15186,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C263"/>
   <sheetViews>
@@ -17740,4 +17472,273 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>1455</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="26" t="s">
+        <v>1177</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>1179</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="26" t="s">
+        <v>224</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>235</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="26" t="s">
+        <v>236</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="26" t="s">
+        <v>237</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="26" t="s">
+        <v>238</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>1411</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>1413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>1410</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>1415</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>1419</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>1420</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
20170909T1330 - References answers.
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -7845,7 +7845,7 @@
   </sheetPr>
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -14389,9 +14389,7 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
20170910T2024 - ToC content completed! Ready for final review!
</commit_message>
<xml_diff>
--- a/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
+++ b/docs/src/main/asciidoc/dist/cl/xlsx/ESPD-CodeLists-V02.00.00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" activeTab="6"/>
+    <workbookView xWindow="7275" yWindow="1575" windowWidth="12630" windowHeight="6420" tabRatio="884" firstSheet="16" activeTab="23"/>
   </bookViews>
   <sheets>
     <sheet name="ActivityType" sheetId="155" r:id="rId1"/>
@@ -9309,7 +9309,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -10883,8 +10883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B35"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14389,7 +14389,7 @@
   </sheetPr>
   <dimension ref="A1:D74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>